<commit_message>
added dotenv and Doors and windows schedules to env and assets folders
</commit_message>
<xml_diff>
--- a/boq_output.xlsx
+++ b/boq_output.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,927 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>BESMM4 Work Sections Master Bill</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in A A 542</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in A A 542</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>29.34</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in A A 542</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in A A 542</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>10.48</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in madam's 3125 bedroom D4 master's W1 0085 0794 0755 009 0051</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in madam's 3125 bedroom D4 master's W1 0085 0794 0755 009 0051</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>21.95</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in madam's 3125 bedroom D4 master's W1 0085 0794 0755 009 0051</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in madam's 3125 bedroom D4 master's W1 0085 0794 0755 009 0051</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>7.84</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in DINING 0081 5253 5591</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>29.37</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in DINING 0081 5253 5591</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>60.73</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in DINING 0081 5253 5591</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>29.37</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in DINING 0081 5253 5591</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>21.69</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in ent. MAIN LIVING 5525 5842 5845</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>32.28</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in ent. MAIN LIVING 5525 5842 5845</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>63.64</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in ent. MAIN LIVING 5525 5842 5845</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>32.28</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in ent. MAIN LIVING 5525 5842 5845</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>22.73</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in D D3 D3 D 09121 0311 076 09121</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>83.19</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in D D3 D3 D 09121 0311 076 09121</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>102.14</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in D D3 D3 D 09121 0311 076 09121</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>83.19</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in D D3 D3 D 09121 0311 076 09121</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>36.48</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in E E</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>31.05</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in E E</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in E E</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>31.05</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in E E</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>22.57</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in F c bh edil rd or oe mn ' 1s c bh edil rd or oe mn ' 2s ki 3t 3c 0h 0en 2250 F 0344 0081 0024 0024 0024 0481</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in F c bh edil rd or oe mn ' 1s c bh edil rd or oe mn ' 2s ki 3t 3c 0h 0en 2250 F 0344 0081 0024 0024 0024 0481</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>15.85</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in F c bh edil rd or oe mn ' 1s c bh edil rd or oe mn ' 2s ki 3t 3c 0h 0en 2250 F 0344 0081 0024 0024 0024 0481</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in F c bh edil rd or oe mn ' 1s c bh edil rd or oe mn ' 2s ki 3t 3c 0h 0en 2250 F 0344 0081 0024 0024 0024 0481</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in G 4100 bath bath 4155 G</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>17.04</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in G 4100 bath bath 4155 G</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>46.23</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in G 4100 bath bath 4155 G</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>17.04</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in G 4100 bath bath 4155 G</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>16.51</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in H H</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in H H</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>18.09</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in H H</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in H H</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>6.46</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>600x600mm ceramic tiles laid to floor in CHIKUN L.GA, KADUNA STATE Race Course, Kaduna - Nigeria.</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Emulsion paint on walls in CHIKUN L.GA, KADUNA STATE Race Course, Kaduna - Nigeria.</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>37.02</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>P.O.P suspended ceiling in CHIKUN L.GA, KADUNA STATE Race Course, Kaduna - Nigeria.</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Finishes</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>100mm high ceramic tile skirting in CHIKUN L.GA, KADUNA STATE Race Course, Kaduna - Nigeria.</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>13.22</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>